<commit_message>
wls excel has been modified with new prefix
</commit_message>
<xml_diff>
--- a/wl_mpi_template_v2.xlsx
+++ b/wl_mpi_template_v2.xlsx
@@ -817,9 +817,6 @@
     <t>ocid1.compartment.oc1..aaaaaaaawt3pfvwwsfqcvmn2xgvk5j6yqjvinyk2lcukp2luffymupxqkxva</t>
   </si>
   <si>
-    <t>j2ee</t>
-  </si>
-  <si>
     <t>ocid1.vaultsecret.oc1.eu-frankfurt-1.amaaaaaaretfhzqaouxt73iz6tisrou66oohfyuthvbzuykp6k343jcwxttq</t>
   </si>
   <si>
@@ -839,6 +836,9 @@
   </si>
   <si>
     <t>eu-frankfurt-1</t>
+  </si>
+  <si>
+    <t>j2ee-nonjrf</t>
   </si>
 </sst>
 </file>
@@ -1300,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1380,7 +1380,7 @@
         <v>116</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1403,7 +1403,7 @@
         <v>117</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="19" x14ac:dyDescent="0.35">
@@ -1426,7 +1426,7 @@
         <v>118</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="19" x14ac:dyDescent="0.35">
@@ -1449,7 +1449,7 @@
         <v>119</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -1730,7 +1730,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -2054,7 +2054,7 @@
         <v>138</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -2130,7 +2130,7 @@
         <v>140</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -2217,24 +2217,27 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A18:A19"/>
@@ -2244,22 +2247,19 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F7" r:id="rId1" location="GUID-C543E630-2BBB-49C5-9E73-1E25DBCB8489__NOTE" display="https://docs.oracle.com/en/cloud/paas/weblogic-cloud/scripts/variables-terraform-scripts.html - GUID-C543E630-2BBB-49C5-9E73-1E25DBCB8489__NOTE"/>
@@ -3620,16 +3620,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
     <mergeCell ref="A46:A50"/>
     <mergeCell ref="B46:B50"/>
     <mergeCell ref="C46:C50"/>
     <mergeCell ref="D46:D50"/>
     <mergeCell ref="E46:E50"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
wls mpi excel has been modified with new wls prefix
</commit_message>
<xml_diff>
--- a/wl_mpi_template_v2.xlsx
+++ b/wl_mpi_template_v2.xlsx
@@ -838,7 +838,7 @@
     <t>eu-frankfurt-1</t>
   </si>
   <si>
-    <t>j2ee_nonjrf</t>
+    <t>wls01</t>
   </si>
 </sst>
 </file>
@@ -2222,19 +2222,22 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A18:A19"/>
@@ -2244,22 +2247,19 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F7" r:id="rId1" location="GUID-C543E630-2BBB-49C5-9E73-1E25DBCB8489__NOTE" display="https://docs.oracle.com/en/cloud/paas/weblogic-cloud/scripts/variables-terraform-scripts.html - GUID-C543E630-2BBB-49C5-9E73-1E25DBCB8489__NOTE"/>
@@ -3620,16 +3620,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
     <mergeCell ref="A46:A50"/>
     <mergeCell ref="B46:B50"/>
     <mergeCell ref="C46:C50"/>
     <mergeCell ref="D46:D50"/>
     <mergeCell ref="E46:E50"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
wls-mpi excel has been modified with new wls prefix
</commit_message>
<xml_diff>
--- a/wl_mpi_template_v2.xlsx
+++ b/wl_mpi_template_v2.xlsx
@@ -838,7 +838,7 @@
     <t>eu-frankfurt-1</t>
   </si>
   <si>
-    <t>wls01</t>
+    <t>wls02</t>
   </si>
 </sst>
 </file>
@@ -2222,6 +2222,35 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="D22:D23"/>
@@ -2231,35 +2260,6 @@
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F7" r:id="rId1" location="GUID-C543E630-2BBB-49C5-9E73-1E25DBCB8489__NOTE" display="https://docs.oracle.com/en/cloud/paas/weblogic-cloud/scripts/variables-terraform-scripts.html - GUID-C543E630-2BBB-49C5-9E73-1E25DBCB8489__NOTE"/>
@@ -3620,16 +3620,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="C46:C50"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="E46:E50"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="E23:E24"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="C46:C50"/>
-    <mergeCell ref="D46:D50"/>
-    <mergeCell ref="E46:E50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
wls-mpi excel has been modified with new wls-prefix
</commit_message>
<xml_diff>
--- a/wl_mpi_template_v2.xlsx
+++ b/wl_mpi_template_v2.xlsx
@@ -838,7 +838,7 @@
     <t>eu-frankfurt-1</t>
   </si>
   <si>
-    <t>wls02</t>
+    <t>wls03</t>
   </si>
 </sst>
 </file>
@@ -2222,19 +2222,22 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A18:A19"/>
@@ -2244,22 +2247,19 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F7" r:id="rId1" location="GUID-C543E630-2BBB-49C5-9E73-1E25DBCB8489__NOTE" display="https://docs.oracle.com/en/cloud/paas/weblogic-cloud/scripts/variables-terraform-scripts.html - GUID-C543E630-2BBB-49C5-9E73-1E25DBCB8489__NOTE"/>
@@ -3620,16 +3620,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
     <mergeCell ref="A46:A50"/>
     <mergeCell ref="B46:B50"/>
     <mergeCell ref="C46:C50"/>
     <mergeCell ref="D46:D50"/>
     <mergeCell ref="E46:E50"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
wls-mpi excel has been modified/updated with new wls-prefix
</commit_message>
<xml_diff>
--- a/wl_mpi_template_v2.xlsx
+++ b/wl_mpi_template_v2.xlsx
@@ -838,7 +838,7 @@
     <t>eu-frankfurt-1</t>
   </si>
   <si>
-    <t>wls03</t>
+    <t>wls04</t>
   </si>
 </sst>
 </file>
@@ -2222,6 +2222,35 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="D22:D23"/>
@@ -2231,35 +2260,6 @@
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F7" r:id="rId1" location="GUID-C543E630-2BBB-49C5-9E73-1E25DBCB8489__NOTE" display="https://docs.oracle.com/en/cloud/paas/weblogic-cloud/scripts/variables-terraform-scripts.html - GUID-C543E630-2BBB-49C5-9E73-1E25DBCB8489__NOTE"/>
@@ -3620,16 +3620,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="C46:C50"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="E46:E50"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="E23:E24"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="C46:C50"/>
-    <mergeCell ref="D46:D50"/>
-    <mergeCell ref="E46:E50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
wls mpi excel has been modified/updated with new wls02 prefix
</commit_message>
<xml_diff>
--- a/wl_mpi_template_v2.xlsx
+++ b/wl_mpi_template_v2.xlsx
@@ -838,7 +838,7 @@
     <t>eu-frankfurt-1</t>
   </si>
   <si>
-    <t>wls04</t>
+    <t>wls02</t>
   </si>
 </sst>
 </file>
@@ -2222,19 +2222,22 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A18:A19"/>
@@ -2244,22 +2247,19 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F7" r:id="rId1" location="GUID-C543E630-2BBB-49C5-9E73-1E25DBCB8489__NOTE" display="https://docs.oracle.com/en/cloud/paas/weblogic-cloud/scripts/variables-terraform-scripts.html - GUID-C543E630-2BBB-49C5-9E73-1E25DBCB8489__NOTE"/>
@@ -3620,16 +3620,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
     <mergeCell ref="A46:A50"/>
     <mergeCell ref="B46:B50"/>
     <mergeCell ref="C46:C50"/>
     <mergeCell ref="D46:D50"/>
     <mergeCell ref="E46:E50"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
wls mpi excel has been modified/updated with new wls03 prefix
</commit_message>
<xml_diff>
--- a/wl_mpi_template_v2.xlsx
+++ b/wl_mpi_template_v2.xlsx
@@ -838,7 +838,7 @@
     <t>eu-frankfurt-1</t>
   </si>
   <si>
-    <t>wls02</t>
+    <t>wls03</t>
   </si>
 </sst>
 </file>
@@ -2222,6 +2222,35 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="D22:D23"/>
@@ -2231,35 +2260,6 @@
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F7" r:id="rId1" location="GUID-C543E630-2BBB-49C5-9E73-1E25DBCB8489__NOTE" display="https://docs.oracle.com/en/cloud/paas/weblogic-cloud/scripts/variables-terraform-scripts.html - GUID-C543E630-2BBB-49C5-9E73-1E25DBCB8489__NOTE"/>
@@ -3620,16 +3620,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="C46:C50"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="E46:E50"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="E23:E24"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="C46:C50"/>
-    <mergeCell ref="D46:D50"/>
-    <mergeCell ref="E46:E50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
wls mpi excel has been modified/updated with new wls02 prefix again
</commit_message>
<xml_diff>
--- a/wl_mpi_template_v2.xlsx
+++ b/wl_mpi_template_v2.xlsx
@@ -838,7 +838,7 @@
     <t>eu-frankfurt-1</t>
   </si>
   <si>
-    <t>wls03</t>
+    <t>wls02</t>
   </si>
 </sst>
 </file>
@@ -2222,19 +2222,22 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A18:A19"/>
@@ -2244,22 +2247,19 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F7" r:id="rId1" location="GUID-C543E630-2BBB-49C5-9E73-1E25DBCB8489__NOTE" display="https://docs.oracle.com/en/cloud/paas/weblogic-cloud/scripts/variables-terraform-scripts.html - GUID-C543E630-2BBB-49C5-9E73-1E25DBCB8489__NOTE"/>
@@ -3620,16 +3620,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
     <mergeCell ref="A46:A50"/>
     <mergeCell ref="B46:B50"/>
     <mergeCell ref="C46:C50"/>
     <mergeCell ref="D46:D50"/>
     <mergeCell ref="E46:E50"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>